<commit_message>
Modifications : Sambot_Int_Test.xlsx Sambot_Sys_Test.xlsx Sambot_Unit_Test.xlsx Software Architectural Design Requirements.docx System requirements.docx
</commit_message>
<xml_diff>
--- a/Sambot_Int_Test.xlsx
+++ b/Sambot_Int_Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\OneDrive - ESIGELEC\2A\Méthode et Outils pour la Qalité Logicielle\GIT\SamBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8F52EEA-F310-4241-8DE7-4E81746C11A5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CF8DB0B-5C5A-40C8-BE6B-9F7EA968EF4F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12915" yWindow="4710" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="57">
   <si>
     <t>Detailed Design Requirements</t>
   </si>
@@ -123,10 +123,82 @@
     <t>IT_00700</t>
   </si>
   <si>
-    <t>Ultrason sensor returns a value under</t>
-  </si>
-  <si>
-    <t>Test if the ultrason sensor considered that it detects an obstacle</t>
+    <t>Test if the ultrason sensor considered that it detects an obstacle under 8cm</t>
+  </si>
+  <si>
+    <t>Test if the servomotor rotate in range of [+45°;-45°]</t>
+  </si>
+  <si>
+    <t>Test if the infrared sensor considered that it detects a hole over 4cm</t>
+  </si>
+  <si>
+    <t>HLR_00500</t>
+  </si>
+  <si>
+    <t>HLR_00510</t>
+  </si>
+  <si>
+    <t>IT_00500</t>
+  </si>
+  <si>
+    <t>IT_00510</t>
+  </si>
+  <si>
+    <t>Test if informations are sent by the user to MSP430G2553 with UART</t>
+  </si>
+  <si>
+    <t>Test if informations are sent by the MSP430G2553 to user with UART</t>
+  </si>
+  <si>
+    <t>Test if informations are sent by the MSP430G2553 to MSP430G2231 with SPI</t>
+  </si>
+  <si>
+    <t>Test if informations are sent by the MSP430G2231 to MSP430G2553 with SPI</t>
+  </si>
+  <si>
+    <t>IT_00501</t>
+  </si>
+  <si>
+    <t>IT_00511</t>
+  </si>
+  <si>
+    <t>Test if the bot start when the command is sent</t>
+  </si>
+  <si>
+    <t>Test if the bot stop when the command is sent</t>
+  </si>
+  <si>
+    <t>Test if sensors data are display when user send command</t>
+  </si>
+  <si>
+    <t>Ultrason sensor returns 1 (obstacle detected)</t>
+  </si>
+  <si>
+    <t>Infrared sensor returns 1 (hole detected)</t>
+  </si>
+  <si>
+    <t>Servomotor rotate in range of [+45°;-45°]</t>
+  </si>
+  <si>
+    <t>User receive informations sent by the MSP430G2553</t>
+  </si>
+  <si>
+    <t>MSP430G2553 receive informations sent but the user</t>
+  </si>
+  <si>
+    <t>MSP430G2231 receive the informations sent by the MSP430G2553</t>
+  </si>
+  <si>
+    <t>MSP430G2553 receive the informations sent by the MSP430G2231</t>
+  </si>
+  <si>
+    <t>The bot start</t>
+  </si>
+  <si>
+    <t>The bot stop</t>
+  </si>
+  <si>
+    <t>Sensors data are display</t>
   </si>
 </sst>
 </file>
@@ -183,7 +255,28 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="11">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -222,15 +315,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{15256A83-394A-428D-A7BC-A80D43FB49E7}" name="Tableau1" displayName="Tableau1" ref="A1:F10" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F10" xr:uid="{2991FC0F-3E0C-4893-B79A-AE9CB9605A44}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{15256A83-394A-428D-A7BC-A80D43FB49E7}" name="Tableau1" displayName="Tableau1" ref="A1:F14" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="A1:F14" xr:uid="{2991FC0F-3E0C-4893-B79A-AE9CB9605A44}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{DD7A0286-1FFB-454E-99AE-A762B81365E2}" name="Detailed Design Requirements" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{FBB99E28-0159-4D49-89A8-E463CAF15B70}" name="Test Identifier" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{D0E2BF31-1E96-4685-B5C7-9550E49A8309}" name="Test description" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{E840EC89-E87A-459D-B529-2AB033AAD747}" name="Datas input" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{20985630-5670-4F81-B446-24E4659C0134}" name="Datas excpected output" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{F7D2E23F-A373-4F59-9B54-5D5536343886}" name="Pass/Fail" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{DD7A0286-1FFB-454E-99AE-A762B81365E2}" name="Detailed Design Requirements" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{FBB99E28-0159-4D49-89A8-E463CAF15B70}" name="Test Identifier" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{D0E2BF31-1E96-4685-B5C7-9550E49A8309}" name="Test description" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{E840EC89-E87A-459D-B529-2AB033AAD747}" name="Datas input" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{20985630-5670-4F81-B446-24E4659C0134}" name="Datas excpected output" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{F7D2E23F-A373-4F59-9B54-5D5536343886}" name="Pass/Fail" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -499,15 +592,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="33.28515625" customWidth="1"/>
+    <col min="1" max="4" width="33.28515625" customWidth="1"/>
+    <col min="5" max="5" width="38.140625" customWidth="1"/>
+    <col min="6" max="6" width="33.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -588,104 +683,156 @@
         <v>25</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+      <c r="E6" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="1"/>
+      <c r="C7" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
+      <c r="E7" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="C12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="C13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="C14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -880,8 +1027,48 @@
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
     </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="F2:F14">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",F2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",F2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
Modifications : Sambot_Int_Test.xlsx Sambot_Sys_Test.xlsx Sambot_Unit_Test.xlsx Software Detailed Design Requirements.docx
</commit_message>
<xml_diff>
--- a/Sambot_Int_Test.xlsx
+++ b/Sambot_Int_Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\OneDrive - ESIGELEC\2A\Méthode et Outils pour la Qalité Logicielle\GIT\SamBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CF8DB0B-5C5A-40C8-BE6B-9F7EA968EF4F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8E0F2D5-B81D-4D64-B8B2-AD7B8094AAF4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="66">
   <si>
     <t>Detailed Design Requirements</t>
   </si>
@@ -43,162 +43,237 @@
   </si>
   <si>
     <t>Pass/Fail</t>
+  </si>
+  <si>
+    <t>HLR_00100</t>
+  </si>
+  <si>
+    <t>HLR_00200</t>
+  </si>
+  <si>
+    <t>HLR_00210</t>
+  </si>
+  <si>
+    <t>HLR_00300</t>
+  </si>
+  <si>
+    <t>HLR_00600</t>
+  </si>
+  <si>
+    <t>HLR_00610</t>
+  </si>
+  <si>
+    <t>HLR_00700</t>
+  </si>
+  <si>
+    <t>HLR_00110</t>
+  </si>
+  <si>
+    <t>HLR_00120</t>
+  </si>
+  <si>
+    <t>IT_00100</t>
+  </si>
+  <si>
+    <t>IT_00110</t>
+  </si>
+  <si>
+    <t>IT_00120</t>
+  </si>
+  <si>
+    <t>The bot shall move forward</t>
+  </si>
+  <si>
+    <t>The bot shall turn 90°</t>
+  </si>
+  <si>
+    <t>The bot shall turn 180°</t>
+  </si>
+  <si>
+    <t>Test if the bot turn 180° when a hole is detected</t>
+  </si>
+  <si>
+    <t>Test if the bot turn 90° right when an obstacle is detected</t>
+  </si>
+  <si>
+    <t>IT_00200</t>
+  </si>
+  <si>
+    <t>IT_00210</t>
+  </si>
+  <si>
+    <t>IT_00300</t>
+  </si>
+  <si>
+    <t>IT_00600</t>
+  </si>
+  <si>
+    <t>IT_00610</t>
+  </si>
+  <si>
+    <t>IT_00700</t>
+  </si>
+  <si>
+    <t>Test if the ultrason sensor considered that it detects an obstacle under 8cm</t>
+  </si>
+  <si>
+    <t>Test if the servomotor rotate in range of [+45°;-45°]</t>
+  </si>
+  <si>
+    <t>Test if the infrared sensor considered that it detects a hole over 4cm</t>
+  </si>
+  <si>
+    <t>HLR_00500</t>
+  </si>
+  <si>
+    <t>HLR_00510</t>
+  </si>
+  <si>
+    <t>IT_00500</t>
+  </si>
+  <si>
+    <t>IT_00510</t>
+  </si>
+  <si>
+    <t>Test if informations are sent by the user to MSP430G2553 with UART</t>
+  </si>
+  <si>
+    <t>Test if informations are sent by the MSP430G2553 to user with UART</t>
+  </si>
+  <si>
+    <t>Test if informations are sent by the MSP430G2553 to MSP430G2231 with SPI</t>
+  </si>
+  <si>
+    <t>Test if informations are sent by the MSP430G2231 to MSP430G2553 with SPI</t>
+  </si>
+  <si>
+    <t>IT_00501</t>
+  </si>
+  <si>
+    <t>IT_00511</t>
+  </si>
+  <si>
+    <t>Test if the bot start when the command is sent</t>
+  </si>
+  <si>
+    <t>Test if the bot stop when the command is sent</t>
+  </si>
+  <si>
+    <t>Test if sensors data are display when user send command</t>
+  </si>
+  <si>
+    <t>Ultrason sensor returns 1 (obstacle detected)</t>
+  </si>
+  <si>
+    <t>Infrared sensor returns 1 (hole detected)</t>
+  </si>
+  <si>
+    <t>Servomotor rotate in range of [+45°;-45°]</t>
+  </si>
+  <si>
+    <t>User receive informations sent by the MSP430G2553</t>
+  </si>
+  <si>
+    <t>MSP430G2553 receive informations sent but the user</t>
+  </si>
+  <si>
+    <t>MSP430G2231 receive the informations sent by the MSP430G2553</t>
+  </si>
+  <si>
+    <t>MSP430G2553 receive the informations sent by the MSP430G2231</t>
+  </si>
+  <si>
+    <t>The bot start</t>
+  </si>
+  <si>
+    <t>The bot stop</t>
+  </si>
+  <si>
+    <t>Sensors data are display</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>Test if the bot move forward when the user turn on autopilote mode</t>
+  </si>
+  <si>
+    <t>1
+0
+2
+4
+6</t>
+  </si>
+  <si>
+    <t>1
+0
+2
+3
+4
+5
+6</t>
+  </si>
+  <si>
+    <t>2
+4
+6
+8
+10
+12
+30</t>
   </si>
   <si>
     <t>0
 1
 2
-a</t>
-  </si>
-  <si>
-    <t>HLR_00100</t>
-  </si>
-  <si>
-    <t>HLR_00200</t>
-  </si>
-  <si>
-    <t>HLR_00210</t>
-  </si>
-  <si>
-    <t>HLR_00300</t>
-  </si>
-  <si>
-    <t>HLR_00600</t>
-  </si>
-  <si>
-    <t>HLR_00610</t>
-  </si>
-  <si>
-    <t>HLR_00700</t>
-  </si>
-  <si>
-    <t>HLR_00110</t>
-  </si>
-  <si>
-    <t>HLR_00120</t>
-  </si>
-  <si>
-    <t>IT_00100</t>
-  </si>
-  <si>
-    <t>IT_00110</t>
-  </si>
-  <si>
-    <t>IT_00120</t>
-  </si>
-  <si>
-    <t>The bot shall move forward</t>
-  </si>
-  <si>
-    <t>The bot shall turn 90°</t>
-  </si>
-  <si>
-    <t>The bot shall turn 180°</t>
-  </si>
-  <si>
-    <t>Test if the bot move forward when the user turn the bot on</t>
-  </si>
-  <si>
-    <t>Test if the bot turn 180° when a hole is detected</t>
-  </si>
-  <si>
-    <t>Test if the bot turn 90° right when an obstacle is detected</t>
-  </si>
-  <si>
-    <t>IT_00200</t>
-  </si>
-  <si>
-    <t>IT_00210</t>
-  </si>
-  <si>
-    <t>IT_00300</t>
-  </si>
-  <si>
-    <t>IT_00600</t>
-  </si>
-  <si>
-    <t>IT_00610</t>
-  </si>
-  <si>
-    <t>IT_00700</t>
-  </si>
-  <si>
-    <t>Test if the ultrason sensor considered that it detects an obstacle under 8cm</t>
-  </si>
-  <si>
-    <t>Test if the servomotor rotate in range of [+45°;-45°]</t>
-  </si>
-  <si>
-    <t>Test if the infrared sensor considered that it detects a hole over 4cm</t>
-  </si>
-  <si>
-    <t>HLR_00500</t>
-  </si>
-  <si>
-    <t>HLR_00510</t>
-  </si>
-  <si>
-    <t>IT_00500</t>
-  </si>
-  <si>
-    <t>IT_00510</t>
-  </si>
-  <si>
-    <t>Test if informations are sent by the user to MSP430G2553 with UART</t>
-  </si>
-  <si>
-    <t>Test if informations are sent by the MSP430G2553 to user with UART</t>
-  </si>
-  <si>
-    <t>Test if informations are sent by the MSP430G2553 to MSP430G2231 with SPI</t>
-  </si>
-  <si>
-    <t>Test if informations are sent by the MSP430G2231 to MSP430G2553 with SPI</t>
-  </si>
-  <si>
-    <t>IT_00501</t>
-  </si>
-  <si>
-    <t>IT_00511</t>
-  </si>
-  <si>
-    <t>Test if the bot start when the command is sent</t>
-  </si>
-  <si>
-    <t>Test if the bot stop when the command is sent</t>
-  </si>
-  <si>
-    <t>Test if sensors data are display when user send command</t>
-  </si>
-  <si>
-    <t>Ultrason sensor returns 1 (obstacle detected)</t>
-  </si>
-  <si>
-    <t>Infrared sensor returns 1 (hole detected)</t>
-  </si>
-  <si>
-    <t>Servomotor rotate in range of [+45°;-45°]</t>
-  </si>
-  <si>
-    <t>User receive informations sent by the MSP430G2553</t>
-  </si>
-  <si>
-    <t>MSP430G2553 receive informations sent but the user</t>
-  </si>
-  <si>
-    <t>MSP430G2231 receive the informations sent by the MSP430G2553</t>
-  </si>
-  <si>
-    <t>MSP430G2553 receive the informations sent by the MSP430G2231</t>
-  </si>
-  <si>
-    <t>The bot start</t>
-  </si>
-  <si>
-    <t>The bot stop</t>
-  </si>
-  <si>
-    <t>Sensors data are display</t>
+4
+8
+10
+30</t>
+  </si>
+  <si>
+    <t>0
+1
+2
+3
+z
+q
+s
+d
+l
+m</t>
+  </si>
+  <si>
+    <t>x
+w
+z
+0
+2
+8</t>
+  </si>
+  <si>
+    <t>6
+4
+10
+20
+50
+70</t>
+  </si>
+  <si>
+    <t>0
+1
+2
+3
+4
+5</t>
+  </si>
+  <si>
+    <t>3
+2
+1
+0
+m
+l</t>
   </si>
 </sst>
 </file>
@@ -255,28 +330,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="10">
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -301,6 +355,20 @@
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -315,15 +383,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{15256A83-394A-428D-A7BC-A80D43FB49E7}" name="Tableau1" displayName="Tableau1" ref="A1:F14" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{15256A83-394A-428D-A7BC-A80D43FB49E7}" name="Tableau1" displayName="Tableau1" ref="A1:F14" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="A1:F14" xr:uid="{2991FC0F-3E0C-4893-B79A-AE9CB9605A44}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{DD7A0286-1FFB-454E-99AE-A762B81365E2}" name="Detailed Design Requirements" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{FBB99E28-0159-4D49-89A8-E463CAF15B70}" name="Test Identifier" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{D0E2BF31-1E96-4685-B5C7-9550E49A8309}" name="Test description" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{E840EC89-E87A-459D-B529-2AB033AAD747}" name="Datas input" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{20985630-5670-4F81-B446-24E4659C0134}" name="Datas excpected output" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{F7D2E23F-A373-4F59-9B54-5D5536343886}" name="Pass/Fail" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{DD7A0286-1FFB-454E-99AE-A762B81365E2}" name="Detailed Design Requirements" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{FBB99E28-0159-4D49-89A8-E463CAF15B70}" name="Test Identifier" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{D0E2BF31-1E96-4685-B5C7-9550E49A8309}" name="Test description" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{E840EC89-E87A-459D-B529-2AB033AAD747}" name="Datas input" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{20985630-5670-4F81-B446-24E4659C0134}" name="Datas excpected output" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{F7D2E23F-A373-4F59-9B54-5D5536343886}" name="Pass/Fail" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -594,8 +662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -625,215 +693,265 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="1" t="s">
+      <c r="C6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="D7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="1" t="s">
+      <c r="C12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B11" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1" t="s">
+      <c r="D13" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="1" t="s">
+      <c r="F13" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="1" t="s">
+      <c r="D14" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F14" s="1"/>
+      <c r="F14" s="1" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
@@ -1062,10 +1180,10 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="F2:F14">
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="9" priority="2" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="8" priority="1" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",F2)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>